<commit_message>
przekonfigurowane karty do najnowszej wersji hardware
</commit_message>
<xml_diff>
--- a/Dokumentacja/zakresy_wersja_3.xlsx
+++ b/Dokumentacja/zakresy_wersja_3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Div1 Mux 1</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>zakres</t>
+  </si>
+  <si>
+    <t>1/wzm RMS</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J8"/>
+  <dimension ref="A3:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +408,7 @@
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -430,8 +433,11 @@
       <c r="J3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.3</v>
       </c>
@@ -461,8 +467,12 @@
         <f>H4/G4</f>
         <v>32.936507936507937</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f>1/I4</f>
+        <v>3.0204778156996581E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -485,15 +495,19 @@
         <v>18.600000000000001</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I18" si="0">F5/E5</f>
+        <f t="shared" ref="I5:I8" si="0">F5/E5</f>
         <v>3.3367346938775513</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J18" si="1">H5/G5</f>
+        <f t="shared" ref="J5:J8" si="1">H5/G5</f>
         <v>3.3453237410071948</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" ref="L5:L8" si="2">1/I5</f>
+        <v>0.29969418960244648</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1000</v>
       </c>
@@ -523,8 +537,12 @@
         <f t="shared" si="1"/>
         <v>1.1734693877551021E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>89.102564102564102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>30</v>
       </c>
@@ -554,8 +572,12 @@
         <f t="shared" si="1"/>
         <v>0.38317757009345788</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>2.6347826086956521</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>300</v>
       </c>
@@ -584,6 +606,50 @@
       <c r="J8">
         <f t="shared" si="1"/>
         <v>3.6530612244897953E-2</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>27.951807228915662</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.3</v>
+      </c>
+      <c r="B12">
+        <v>3.0204778156996601E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>0.29969418960244598</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1000</v>
+      </c>
+      <c r="B14">
+        <v>89.102564102564102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>2.6347826086956498</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>300</v>
+      </c>
+      <c r="B16">
+        <v>27.951807228915701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodano wczytywanie wzmocnień dla każdego kanału oddzielnie odpowiada za to plik konfiguracyjny Katry_AI.ini tabela wzmocnień dla każdego kanału ma rozmiar 8x5
</commit_message>
<xml_diff>
--- a/Dokumentacja/zakresy_wersja_3.xlsx
+++ b/Dokumentacja/zakresy_wersja_3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>Div1 Mux 1</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>1/wzm RMS</t>
+  </si>
+  <si>
+    <t>x5</t>
   </si>
 </sst>
 </file>
@@ -397,18 +400,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L16"/>
+  <dimension ref="A3:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -433,11 +437,14 @@
       <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.3</v>
       </c>
@@ -468,11 +475,23 @@
         <v>32.936507936507937</v>
       </c>
       <c r="L4">
+        <f>I4/5</f>
+        <v>6.621468926553673</v>
+      </c>
+      <c r="M4">
+        <f>1/L4</f>
+        <v>0.15102389078498291</v>
+      </c>
+      <c r="O4">
         <f>1/I4</f>
         <v>3.0204778156996581E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <f>O4*5</f>
+        <v>0.15102389078498291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -503,11 +522,23 @@
         <v>3.3453237410071948</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L8" si="2">1/I5</f>
+        <f t="shared" ref="L5:L8" si="2">I5/5</f>
+        <v>0.66734693877551021</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:M8" si="3">1/L5</f>
+        <v>1.4984709480122325</v>
+      </c>
+      <c r="O5">
+        <f>1/I5</f>
         <v>0.29969418960244648</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <f t="shared" ref="P5:P8" si="4">O5*5</f>
+        <v>1.4984709480122325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1000</v>
       </c>
@@ -539,10 +570,22 @@
       </c>
       <c r="L6">
         <f t="shared" si="2"/>
+        <v>2.2446043165467626E-3</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>445.5128205128205</v>
+      </c>
+      <c r="O6">
+        <f>1/I6</f>
         <v>89.102564102564102</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <f t="shared" si="4"/>
+        <v>445.5128205128205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>30</v>
       </c>
@@ -574,10 +617,22 @@
       </c>
       <c r="L7">
         <f t="shared" si="2"/>
+        <v>7.590759075907591E-2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>13.17391304347826</v>
+      </c>
+      <c r="O7">
+        <f>1/I7</f>
         <v>2.6347826086956521</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <f t="shared" si="4"/>
+        <v>13.17391304347826</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>300</v>
       </c>
@@ -609,47 +664,59 @@
       </c>
       <c r="L8">
         <f t="shared" si="2"/>
+        <v>7.1551724137931035E-3</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>139.75903614457832</v>
+      </c>
+      <c r="O8">
+        <f>1/I8</f>
         <v>27.951807228915662</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>139.75903614457832</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.3</v>
       </c>
       <c r="B12">
-        <v>3.0204778156996601E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.15102389078498299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13">
-        <v>0.29969418960244598</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.49847094801223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1000</v>
       </c>
       <c r="B14">
-        <v>89.102564102564102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>445.51282051281999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>30</v>
       </c>
       <c r="B15">
-        <v>2.6347826086956498</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>13.173913043478301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>300</v>
       </c>
       <c r="B16">
-        <v>27.951807228915701</v>
+        <v>139.759036144578</v>
       </c>
     </row>
   </sheetData>
@@ -659,12 +726,237 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B5:Q10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="E6">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="G6">
+        <v>0.09</v>
+      </c>
+      <c r="H6">
+        <v>2.44</v>
+      </c>
+      <c r="I6">
+        <f>F6/E6</f>
+        <v>29.928571428571427</v>
+      </c>
+      <c r="J6">
+        <f>H6/G6</f>
+        <v>27.111111111111111</v>
+      </c>
+      <c r="O6">
+        <f>1/I6</f>
+        <v>3.3412887828162291E-2</v>
+      </c>
+      <c r="Q6">
+        <v>3.0204778156996581E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>3.5</v>
+      </c>
+      <c r="E7">
+        <v>0.254</v>
+      </c>
+      <c r="F7">
+        <v>0.85</v>
+      </c>
+      <c r="G7">
+        <v>0.78</v>
+      </c>
+      <c r="H7">
+        <v>2.5</v>
+      </c>
+      <c r="I7">
+        <f>F7/E7</f>
+        <v>3.3464566929133857</v>
+      </c>
+      <c r="J7">
+        <f>H7/G7</f>
+        <v>3.2051282051282048</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7:O10" si="0">1/I7</f>
+        <v>0.29882352941176471</v>
+      </c>
+      <c r="Q7">
+        <v>0.29969418960244648</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E8">
+        <v>7.23</v>
+      </c>
+      <c r="F8">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G8">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.24</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ref="I8:I10" si="1">F8/E8</f>
+        <v>1.1756569847856155E-2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J10" si="2">H8/G8</f>
+        <v>1.1764705882352941E-2</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>85.058823529411768</v>
+      </c>
+      <c r="Q8">
+        <v>89.102564102564102</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>0.36</v>
+      </c>
+      <c r="E9">
+        <v>2.17</v>
+      </c>
+      <c r="F9">
+        <v>0.84</v>
+      </c>
+      <c r="G9">
+        <v>6.24</v>
+      </c>
+      <c r="H9">
+        <v>2.5</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0.38709677419354838</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>0.40064102564102561</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>2.5833333333333335</v>
+      </c>
+      <c r="Q9">
+        <v>2.6347826086956521</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>300</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E10">
+        <v>7.23</v>
+      </c>
+      <c r="F10">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="G10">
+        <v>20.8</v>
+      </c>
+      <c r="H10">
+        <v>0.76</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>3.6791147994467498E-2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>3.653846153846154E-2</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>27.180451127819548</v>
+      </c>
+      <c r="Q10">
+        <v>27.951807228915662</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>